<commit_message>
契約者別請求一覧 Signed-off-by: LiuYiyang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/test_契約管理/已完成/test_契約管理_随時対応_10解約_契約違反解約.xlsx
+++ b/test_契約管理/已完成/test_契約管理_随時対応_10解約_契約違反解約.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="758" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="758" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IN_DB_001" sheetId="7" r:id="rId1"/>
@@ -14595,8 +14595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:EL35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -30361,7 +30361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CC60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>

</xml_diff>